<commit_message>
adding plots and report
</commit_message>
<xml_diff>
--- a/excel/exp1_train_test.xlsx
+++ b/excel/exp1_train_test.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Frequently Used\Fall 2015\CS760\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\public\food-image-classification\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="exp1_train_test" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -584,1906 +584,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>[1]acc2!$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>20k samples</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="38100" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>[1]acc2!$E$2:$E$57</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="56"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>56</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>[1]acc2!$F$2:$F$57</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="56"/>
-                <c:pt idx="0">
-                  <c:v>15.624997019799999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>14.024998247600001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.999999523200001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>12.1500000358</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11.450002342499999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10.724999755599999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10.049999505300001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.9500010013600004</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8.2000009715599997</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7.3999993503100008</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7.1249991655299993</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>6.8999990820899999</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6.3999995589300003</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6.2499992549400005</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>6.1499994248199998</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>6.0749992728200004</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5.8749988675099996</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5.8499988168500003</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>5.8999985456499999</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>5.8499984443200006</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>5.7499986141899999</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>5.6749988347300002</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>5.6499991565899998</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>5.6499995291199996</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>5.6249998509900001</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>5.6249998509900001</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>5.6000001728499997</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>5.4999999702000002</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>5.4249998182099999</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>5.4249998182099999</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>5.4249998182099999</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>5.3999997675399998</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>5.3999997675399998</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>5.3749997168800006</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>5.3499996662100004</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>5.3499996662100004</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>5.3249996155500003</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>5.3749997168800006</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>5.3749997168800006</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>5.3749997168800006</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>5.3749997168800006</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>5.3749997168800006</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>5.3499996662100004</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>5.3499996662100004</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>5.3499996662100004</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>5.3749997168800006</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>5.3749997168800006</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>5.3999997675399998</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>5.4249998182099999</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>5.4250001907299996</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>5.4250001907299996</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>5.4250001907299996</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>5.3999997675399998</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>5.3999997675399998</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>5.3999997675399998</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>5.3999997675399998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5BA3-4A7C-A5DC-2E52CE4820A4}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>[1]acc2!$G$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>15k samples</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="38100" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>[1]acc2!$E$2:$E$57</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="56"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>56</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>[1]acc2!$G$2:$G$57</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="56"/>
-                <c:pt idx="0">
-                  <c:v>23.824997246300001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>17.399999499300002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.624999880800001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10.5999998748</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.5249995589300003</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8.9250005781699997</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.87499919534</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.34999999404</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7.4500009417499999</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7.4500001967000005</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7.2750009596299998</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>7.6499998569500001</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>7.3749996721700004</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>7.3000013828299997</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7.2999998927100007</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>7.2999998927100007</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>7.34999999404</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>7.3999993503100008</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>7.4749991297700005</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>7.4250005185600001</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>7.4500001967000005</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>7.4500001967000005</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>7.4000000953700003</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>7.3250003159000006</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>7.2249993681899998</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>7.1749992668599996</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>7.0999994873999999</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>7.0749998092699995</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>7.0499993860699997</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>7.0499993860699997</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>7.0249989628799998</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>6.97499960661</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>6.9499999284700005</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>6.8749994039499995</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>6.8999998271499994</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>6.7999996244899998</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>6.7999996244899998</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>6.7499995231599996</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>6.7999996244899998</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>6.7499995231599996</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>6.7249998450300001</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>6.6999994218299994</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>6.6499993205100001</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>6.6249996423699997</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>6.6499993205100001</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>6.3749998807899999</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>6.4000003039799997</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>6.4249999821200001</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>6.4249999821200001</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>6.4249999821200001</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>6.45000040531</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>6.4000003039799997</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>6.3749998807899999</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>6.3500002026600004</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>6.3000001013300002</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>6.25</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5BA3-4A7C-A5DC-2E52CE4820A4}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>[1]acc2!$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>10k samples</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="38100" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>[1]acc2!$E$2:$E$57</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="56"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>56</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>[1]acc2!$H$2:$H$57</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="56"/>
-                <c:pt idx="0">
-                  <c:v>23.649998009199997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13.0750000477</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10.974999517200001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11.3000005484</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10.274998843700001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10.399999469500001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9.799999743699999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.7000002860999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.8249994218300003</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9.6749991178499997</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>8.950000256300001</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>8.6249992251399998</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>8.3750002086199995</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8.1500016152899999</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7.75000080466</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>10.000000149</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>8.6000002920600007</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>8.2499995827700001</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>8.1249997019800002</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>7.9999998211900003</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>7.87499919534</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>7.8249998390700002</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>7.8500010073199995</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>7.77499973774</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>7.8000001609299998</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>7.7999994158700003</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>7.7499993145500001</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>7.7499993145500001</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>7.7249996364099998</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>7.6749995350800004</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>7.5749993324300009</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>7.5749993324300009</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>7.5249992311000007</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>7.4749991297700005</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>7.3999993503100008</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>7.3999993503100008</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>7.4249997735000006</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>7.4749998748299999</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>7.449999451640001</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>7.3999993503100008</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>7.3999993503100008</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>7.3749996721700004</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>7.3749996721700004</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>7.3499992489800006</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>7.3499992489800006</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>7.3499992489800006</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>7.3249995708499993</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>7.3499992489800006</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>7.3499992489800006</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>7.3249995708499993</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>7.3499992489800006</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>7.3499992489800006</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>7.3249995708499993</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>7.34999999404</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>7.34999999404</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>7.34999999404</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-5BA3-4A7C-A5DC-2E52CE4820A4}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>[1]acc2!$I$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>5k samples</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="38100" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>[1]acc2!$E$2:$E$57</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="56"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>56</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>[1]acc2!$I$2:$I$57</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="56"/>
-                <c:pt idx="0">
-                  <c:v>27.750000357600001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>18.875001370899998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15.549997985399999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.149999082100001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>14.3250018358</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>12.0749995112</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12.150000780799999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>11.525000631800001</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>11.450000852300001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11.474998295300001</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10.525000095399999</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>10.500000417200001</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>10.2999992669</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>10.149999707899999</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>10.125000029800001</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>9.9750004708799995</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>9.8249994218300003</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>9.7249984741199995</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>9.6749983727900002</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>9.6249990165200003</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>9.499998390670001</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>9.4749987125399997</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>9.4750002026600004</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>9.474999457600001</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>9.4499990343999993</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>9.375</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>9.275000542399999</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>9.3000002205399994</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>9.275000542399999</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>9.400000423189999</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>9.4249993562699999</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>9.4749987125399997</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>9.4249993562699999</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>9.4249993562699999</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>9.274999052290001</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>9.2499993741500006</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>9.274999052290001</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>9.2499986290900011</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>9.2249982058999986</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>9.1999977827099997</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>9.1499984264399998</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>9.1499991715000011</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>9.1499991715000011</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>9.1249994933600007</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>9.0999998152300012</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>9.1250002384200002</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>9.0750001370900009</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>9.0750001370900009</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>9.0750001370900009</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>9.0500004589599996</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>9.0750001370900009</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>9.1249994933600007</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>9.1249994933600007</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>9.1249994933600007</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>9.1249994933600007</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>9.1499991715000011</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-5BA3-4A7C-A5DC-2E52CE4820A4}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="471492224"/>
-        <c:axId val="471492880"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="471492224"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="55"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="2000"/>
-                  <a:t>Epochs</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="471492880"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-        <c:majorUnit val="5"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="471492880"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="2000"/>
-                  <a:t>Test error</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
-                  <a:t> (%)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" sz="2000"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="471492224"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2530,10 +631,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>exp1_train_test!$D$2:$D$55</c:f>
+              <c:f>exp1_train_test!$D$2:$D$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2695,16 +796,19 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>exp1_train_test!$E$2:$E$55</c:f>
+              <c:f>exp1_train_test!$E$2:$E$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>15.624997019799999</c:v>
                 </c:pt>
@@ -2865,13 +969,16 @@
                   <c:v>5.3999997675399998</c:v>
                 </c:pt>
                 <c:pt idx="53">
+                  <c:v>5.3999997675399998</c:v>
+                </c:pt>
+                <c:pt idx="54">
                   <c:v>5.3999997675399998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-65DD-44F5-9D88-55C72E0C4E9C}"/>
             </c:ext>
@@ -2905,10 +1012,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>exp1_train_test!$D$2:$D$55</c:f>
+              <c:f>exp1_train_test!$D$2:$D$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3070,16 +1177,19 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>exp1_train_test!$F$2:$F$55</c:f>
+              <c:f>exp1_train_test!$F$2:$F$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>13.845004141299999</c:v>
                 </c:pt>
@@ -3240,13 +1350,16 @@
                   <c:v>6.4999994356199992E-2</c:v>
                 </c:pt>
                 <c:pt idx="53">
+                  <c:v>6.4999994356199992E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
                   <c:v>6.4999994356199992E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-65DD-44F5-9D88-55C72E0C4E9C}"/>
             </c:ext>
@@ -3280,10 +1393,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>exp1_train_test!$D$2:$D$55</c:f>
+              <c:f>exp1_train_test!$D$2:$D$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -3445,16 +1558,19 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>exp1_train_test!$G$2:$G$55</c:f>
+              <c:f>exp1_train_test!$G$2:$G$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="55"/>
                 <c:pt idx="0">
                   <c:v>16.1250010133</c:v>
                 </c:pt>
@@ -3616,12 +1732,15 @@
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>5.5749993771300002</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5.4999995976700005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-65DD-44F5-9D88-55C72E0C4E9C}"/>
             </c:ext>
@@ -3635,11 +1754,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="535264592"/>
-        <c:axId val="535263936"/>
+        <c:axId val="915338608"/>
+        <c:axId val="915339168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="535264592"/>
+        <c:axId val="915338608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="55"/>
@@ -3660,6 +1779,20 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -3753,16 +1886,16 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="535263936"/>
+        <c:crossAx val="915339168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="535263936"/>
+        <c:axId val="915339168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="17"/>
+          <c:max val="18"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -3781,6 +1914,20 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -3874,10 +2021,11 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="535264592"/>
+        <c:crossAx val="915338608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="4"/>
+        <c:majorUnit val="2"/>
+        <c:minorUnit val="0.5"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -3957,46 +2105,6 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4552,556 +2660,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>26670</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>125730</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
@@ -5126,7 +2686,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6381,12 +3941,12 @@
   <dimension ref="A1:G102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+      <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6406,7 +3966,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.15624997019799999</v>
       </c>
@@ -6432,7 +3992,7 @@
         <v>16.1250010133</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.14024998247600001</v>
       </c>
@@ -6458,7 +4018,7 @@
         <v>14.374999701999998</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.12999999523200001</v>
       </c>
@@ -6484,7 +4044,7 @@
         <v>13.625000417200001</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.121500000358</v>
       </c>
@@ -6510,7 +4070,7 @@
         <v>12.775000929800001</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.114500023425</v>
       </c>
@@ -6536,7 +4096,7 @@
         <v>12.150000780799999</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.107249997556</v>
       </c>
@@ -6562,7 +4122,7 @@
         <v>11.850000172900002</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.100499995053</v>
       </c>
@@ -6588,7 +4148,7 @@
         <v>11.200000345699999</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8.9500010013600001E-2</v>
       </c>
@@ -6614,7 +4174,7 @@
         <v>10.0500002503</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8.2000009715599995E-2</v>
       </c>
@@ -6640,7 +4200,7 @@
         <v>8.825000375510001</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7.3999993503100006E-2</v>
       </c>
@@ -6666,7 +4226,7 @@
         <v>8.0250002443799993</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>7.1249991655299993E-2</v>
       </c>
@@ -6692,7 +4252,7 @@
         <v>7.5249999761600002</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6.8999990820899998E-2</v>
       </c>
@@ -6718,7 +4278,7 @@
         <v>7.3250003159000006</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6.3999995589300002E-2</v>
       </c>
@@ -6744,7 +4304,7 @@
         <v>6.9000005722000006</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6.2499992549400002E-2</v>
       </c>
@@ -6770,7 +4330,7 @@
         <v>6.5749995410399995</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>6.1499994248199998E-2</v>
       </c>
@@ -6796,7 +4356,7 @@
         <v>6.3499994576000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>6.0749992728200003E-2</v>
       </c>
@@ -6822,7 +4382,7 @@
         <v>6.2499996274700003</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5.87499886751E-2</v>
       </c>
@@ -6848,7 +4408,7 @@
         <v>6.1499994248199998</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5.8499988168500001E-2</v>
       </c>
@@ -6874,7 +4434,7 @@
         <v>5.9499993920299996</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5.8999985456500002E-2</v>
       </c>
@@ -6900,7 +4460,7 @@
         <v>5.9249993413699995</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>5.8499984443200002E-2</v>
       </c>
@@ -6926,7 +4486,7 @@
         <v>5.9249993413699995</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>5.7499986141900002E-2</v>
       </c>
@@ -6952,7 +4512,7 @@
         <v>5.9249997139000001</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>5.6749988347300002E-2</v>
       </c>
@@ -6978,7 +4538,7 @@
         <v>5.9499997645600002</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>5.64999915659E-2</v>
       </c>
@@ -7004,7 +4564,7 @@
         <v>5.9249993413699995</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>5.6499995291199999E-2</v>
       </c>
@@ -7030,7 +4590,7 @@
         <v>5.8499991893800001</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>5.62499985099E-2</v>
       </c>
@@ -7056,7 +4616,7 @@
         <v>5.8499991893800001</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>5.62499985099E-2</v>
       </c>
@@ -7082,7 +4642,7 @@
         <v>5.7999994605799996</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>5.6000001728499997E-2</v>
       </c>
@@ -7108,7 +4668,7 @@
         <v>5.7749990373799998</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>5.4999999702000001E-2</v>
       </c>
@@ -7134,7 +4694,7 @@
         <v>5.7999990880499999</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>5.4249998182100002E-2</v>
       </c>
@@ -7160,7 +4720,7 @@
         <v>5.7249993085900002</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>5.4249998182100002E-2</v>
       </c>
@@ -7186,7 +4746,7 @@
         <v>5.7249993085900002</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>5.4249998182100002E-2</v>
       </c>
@@ -7212,7 +4772,7 @@
         <v>5.7499986141899999</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -7238,7 +4798,7 @@
         <v>5.7249985635300007</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -7264,7 +4824,7 @@
         <v>5.6999985128600006</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>5.3749997168800003E-2</v>
       </c>
@@ -7290,7 +4850,7 @@
         <v>5.6999985128600006</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>5.3499996662100001E-2</v>
       </c>
@@ -7316,7 +4876,7 @@
         <v>5.6749988347300002</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>5.3499996662100001E-2</v>
       </c>
@@ -7342,7 +4902,7 @@
         <v>5.6749988347300002</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>5.3249996155500003E-2</v>
       </c>
@@ -7368,7 +4928,7 @@
         <v>5.6999985128600006</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>5.3749997168800003E-2</v>
       </c>
@@ -7394,7 +4954,7 @@
         <v>5.6749984622000005</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>5.3749997168800003E-2</v>
       </c>
@@ -7420,7 +4980,7 @@
         <v>5.6749988347300002</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>5.3749997168800003E-2</v>
       </c>
@@ -7446,7 +5006,7 @@
         <v>5.6749988347300002</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>5.3749997168800003E-2</v>
       </c>
@@ -7472,7 +5032,7 @@
         <v>5.6999985128600006</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>5.3749997168800003E-2</v>
       </c>
@@ -7498,7 +5058,7 @@
         <v>5.6749984622000005</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>5.3499996662100001E-2</v>
       </c>
@@ -7524,7 +5084,7 @@
         <v>5.6749984622000005</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>5.3499996662100001E-2</v>
       </c>
@@ -7550,7 +5110,7 @@
         <v>5.6499987840700001</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>5.3499996662100001E-2</v>
       </c>
@@ -7576,7 +5136,7 @@
         <v>5.6499987840700001</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>5.3749997168800003E-2</v>
       </c>
@@ -7602,7 +5162,7 @@
         <v>5.5999994278000003</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>5.3749997168800003E-2</v>
       </c>
@@ -7628,7 +5188,7 @@
         <v>5.6249994784600004</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -7654,7 +5214,7 @@
         <v>5.6249994784600004</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>5.4249998182100002E-2</v>
       </c>
@@ -7680,7 +5240,7 @@
         <v>5.6249994784600004</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>5.4250001907299998E-2</v>
       </c>
@@ -7706,7 +5266,7 @@
         <v>5.5999994278000003</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>5.4250001907299998E-2</v>
       </c>
@@ -7732,7 +5292,7 @@
         <v>5.5999994278000003</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>5.4250001907299998E-2</v>
       </c>
@@ -7758,7 +5318,7 @@
         <v>5.54999932647</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -7784,7 +5344,7 @@
         <v>5.5749993771300002</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -7810,7 +5370,7 @@
         <v>5.5749993771300002</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -7836,7 +5396,7 @@
         <v>5.4999995976700005</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -7862,7 +5422,7 @@
         <v>5.4999995976700005</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>5.4249998182100002E-2</v>
       </c>
@@ -7888,7 +5448,7 @@
         <v>5.4999995976700005</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>5.4249998182100002E-2</v>
       </c>
@@ -7914,7 +5474,7 @@
         <v>5.4999995976700005</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>5.4249998182100002E-2</v>
       </c>
@@ -7940,7 +5500,7 @@
         <v>5.5249992757999999</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>5.4249998182100002E-2</v>
       </c>
@@ -7966,7 +5526,7 @@
         <v>5.5249992757999999</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>5.4249998182100002E-2</v>
       </c>
@@ -7992,7 +5552,7 @@
         <v>5.5499989539400003</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -8018,7 +5578,7 @@
         <v>5.5249992757999999</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -8044,7 +5604,7 @@
         <v>5.5249992757999999</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -8070,7 +5630,7 @@
         <v>5.5499989539400003</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -8096,7 +5656,7 @@
         <v>5.5249992757999999</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -8122,7 +5682,7 @@
         <v>5.5249992757999999</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>5.4249998182100002E-2</v>
       </c>
@@ -8148,7 +5708,7 @@
         <v>5.5249992757999999</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -8174,7 +5734,7 @@
         <v>5.4999992251399998</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>5.3999997675400001E-2</v>
       </c>
@@ -8200,7 +5760,7 @@
         <v>5.4999992251399998</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>5.3499996662100001E-2</v>
       </c>
@@ -8226,7 +5786,7 @@
         <v>5.4999992251399998</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>5.3499996662100001E-2</v>
       </c>
@@ -8252,7 +5812,7 @@
         <v>5.5249992757999999</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>5.3499996662100001E-2</v>
       </c>
@@ -8278,7 +5838,7 @@
         <v>5.4999992251399998</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>5.3499996662100001E-2</v>
       </c>
@@ -8304,7 +5864,7 @@
         <v>5.4999992251399998</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>5.2999995648899997E-2</v>
       </c>
@@ -8330,7 +5890,7 @@
         <v>5.4999992251399998</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>5.2999995648899997E-2</v>
       </c>
@@ -8356,7 +5916,7 @@
         <v>5.4999992251399998</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>5.3249999880800002E-2</v>
       </c>
@@ -8382,7 +5942,7 @@
         <v>5.4999992251399998</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>5.2999999374200003E-2</v>
       </c>
@@ -8408,7 +5968,7 @@
         <v>5.4749995470000004</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>5.3249999880800002E-2</v>
       </c>
@@ -8434,7 +5994,7 @@
         <v>5.4749995470000004</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>5.3249996155500003E-2</v>
       </c>
@@ -8460,7 +6020,7 @@
         <v>5.4749995470000004</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>5.2999995648899997E-2</v>
       </c>
@@ -8486,7 +6046,7 @@
         <v>5.4999995976700005</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>5.2999995648899997E-2</v>
       </c>
@@ -8512,7 +6072,7 @@
         <v>5.4999995976700005</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>5.2999995648899997E-2</v>
       </c>
@@ -8538,7 +6098,7 @@
         <v>5.4999995976700005</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -8564,7 +6124,7 @@
         <v>5.4999995976700005</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -8590,7 +6150,7 @@
         <v>5.5249996483299997</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -8616,7 +6176,7 @@
         <v>5.5249996483299997</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>5.3249996155500003E-2</v>
       </c>
@@ -8642,7 +6202,7 @@
         <v>5.5249996483299997</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>5.3249996155500003E-2</v>
       </c>
@@ -8668,7 +6228,7 @@
         <v>5.5249996483299997</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>5.3249996155500003E-2</v>
       </c>
@@ -8694,7 +6254,7 @@
         <v>5.5249996483299997</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -8720,7 +6280,7 @@
         <v>5.5499996989999998</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -8746,7 +6306,7 @@
         <v>5.5499996989999998</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -8772,7 +6332,7 @@
         <v>5.5249996483299997</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -8798,7 +6358,7 @@
         <v>5.5249996483299997</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -8824,7 +6384,7 @@
         <v>5.5499996989999998</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -8850,7 +6410,7 @@
         <v>5.5499996989999998</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -8876,7 +6436,7 @@
         <v>5.5499996989999998</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -8902,7 +6462,7 @@
         <v>5.5499996989999998</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -8928,7 +6488,7 @@
         <v>5.5499996989999998</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -8954,7 +6514,7 @@
         <v>5.5499996989999998</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -8980,7 +6540,7 @@
         <v>5.5749993771300002</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>5.2749995142200003E-2</v>
       </c>
@@ -9006,7 +6566,7 @@
         <v>5.5749993771300002</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>5.2749995142200003E-2</v>
       </c>

</xml_diff>